<commit_message>
comments + journal updated
</commit_message>
<xml_diff>
--- a/journal.xlsx
+++ b/journal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a525b8895717ea45/Documents/University/Διπλωματική/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a525b8895717ea45/Documents/University/ANC-with-NN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{56E94A9C-4AD6-4643-ACF6-2E1233E7601A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5187411-1605-44EF-B01D-72DFB105CEE8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A2EFF7-04ED-4551-80A2-131D056F3876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1968" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Οκτώβριος 2024</t>
   </si>
@@ -97,6 +97,39 @@
   </si>
   <si>
     <t>Re-write whole code (fix implementation errors and misconceptions) - FxLMS</t>
+  </si>
+  <si>
+    <t>Different noise colors</t>
+  </si>
+  <si>
+    <t>Μάρτιος 2025</t>
+  </si>
+  <si>
+    <t>Debugging (code re-writing, smashing head on the wall)</t>
+  </si>
+  <si>
+    <t>Organize code into multiple files, folders, functions, classes</t>
+  </si>
+  <si>
+    <t>Ποιο είναι το ιδανικό kernel size?</t>
+  </si>
+  <si>
+    <t>Ορίσματα στα convolutions (πχ mode)? Scaling? Δεν ξέρω αν τα αποτελέσματα είναι αναμενόμενα (φυσιολογικά) ή όχι</t>
+  </si>
+  <si>
+    <t>Threads για κάθε λειτουργία που θέλω να τρέχει παράλληλα, άπειρα bugs</t>
+  </si>
+  <si>
+    <t>Thread τρέχει παράλληλα</t>
+  </si>
+  <si>
+    <t>Πολλές πηγές με διαφορετικές υλοποιήσεις σε κώδικα - τελικά τι είναι σωστό?</t>
+  </si>
+  <si>
+    <t>Τα αποτελέσματα είναι αναμενόμενα-σωστά?</t>
+  </si>
+  <si>
+    <t>Δυσκολία στο να φτάσω κοντά στις βέλτιστες τιμές των mu, L γιατί πολύ εύκολα με μεγάλες τιμές το σύστημα οδηγείται σε αστάθεια ενώ με μικρές τιμές δεν συγκλίνει τέπο. Σε κάποιες περιπτώσεις ο θόρυβος αυξάνεται, ή η ένταση ξεκινάει από πολύ χαμηλή και αυξάνεται ή παραμένει πολύ χαμηλή</t>
   </si>
 </sst>
 </file>
@@ -158,10 +191,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -429,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,11 +578,13 @@
       <c r="C7" s="2">
         <v>4</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>23</v>
@@ -561,7 +592,9 @@
       <c r="C8" s="2">
         <v>12</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
@@ -577,7 +610,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>19</v>
@@ -585,24 +618,29 @@
       <c r="C10" s="2">
         <v>6</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="2">
         <v>5</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
@@ -621,31 +659,49 @@
       <c r="C13" s="2">
         <v>2</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>

</xml_diff>